<commit_message>
Se hicieron cambios 23112020
</commit_message>
<xml_diff>
--- a/SGA_PCR/Imagenes/Gantt - Software Apolo 20112020.xlsx
+++ b/SGA_PCR/Imagenes/Gantt - Software Apolo 20112020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GitHub\SistemaInventarioPCR\SGA_PCR\Imagenes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1DE3AC-3F26-45DB-8707-904C7BE159D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F717FA-4A33-4299-8B3E-33C4FBA8F21B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11269,10 +11269,10 @@
   <dimension ref="A1:EO34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>